<commit_message>
Made changes to fanconi screener
</commit_message>
<xml_diff>
--- a/src/test/resources/ServiceNow/CHARMS/Resources/data.xlsx
+++ b/src/test/resources/ServiceNow/CHARMS/Resources/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/resources/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721D980F-FE26-844D-ADEB-3798A7976289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31324982-0F7A-BB45-BE06-E562668266A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="520" windowWidth="26000" windowHeight="20280" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="4240" yWindow="760" windowWidth="26000" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="433">
   <si>
     <t>Yes</t>
   </si>
@@ -271,9 +271,6 @@
     <t>Asp23llefs</t>
   </si>
   <si>
-    <t>FANCA</t>
-  </si>
-  <si>
     <t>Eltrobopag</t>
   </si>
   <si>
@@ -505,9 +502,6 @@
     <t>Upload to this questionnaire</t>
   </si>
   <si>
-    <t>FANCB</t>
-  </si>
-  <si>
     <t>Father</t>
   </si>
   <si>
@@ -568,9 +562,6 @@
     <t>Mail</t>
   </si>
   <si>
-    <t>FANCC</t>
-  </si>
-  <si>
     <t>Don't Know</t>
   </si>
   <si>
@@ -1135,9 +1126,6 @@
     <t>Other Test</t>
   </si>
   <si>
-    <t>FANCD1 (BRCA2)</t>
-  </si>
-  <si>
     <t>11/23/2000</t>
   </si>
   <si>
@@ -1171,9 +1159,6 @@
     <t>Fanconi-Proxy 1</t>
   </si>
   <si>
-    <t>FANCF</t>
-  </si>
-  <si>
     <t>Asp23llefsds</t>
   </si>
   <si>
@@ -1207,9 +1192,6 @@
     <t>charmsparticipant12@yopmail.com</t>
   </si>
   <si>
-    <t>FANCS(BRCA1)</t>
-  </si>
-  <si>
     <t>Gilaterbopager</t>
   </si>
   <si>
@@ -1222,12 +1204,6 @@
     <t>Medication Test 3</t>
   </si>
   <si>
-    <t>FANCL (PHF9/POG)</t>
-  </si>
-  <si>
-    <t>FANCT (UBE2T)</t>
-  </si>
-  <si>
     <t>Cousin</t>
   </si>
   <si>
@@ -1361,6 +1337,9 @@
   </si>
   <si>
     <t>P-9</t>
+  </si>
+  <si>
+    <t>Other genes/syndromes</t>
   </si>
 </sst>
 </file>
@@ -1679,9 +1658,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1719,7 +1698,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1825,7 +1804,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1967,7 +1946,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1980,9 +1959,9 @@
   </sheetPr>
   <dimension ref="A1:EJ18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="113" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="113" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BY2" sqref="BY2:BY13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2043,46 +2022,46 @@
   <sheetData>
     <row r="1" spans="1:140" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>200</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>1</v>
@@ -2094,7 +2073,7 @@
         <v>3</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S1" s="10" t="s">
         <v>4</v>
@@ -2103,16 +2082,16 @@
         <v>5</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="V1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="W1" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="X1" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="Y1" s="7" t="s">
         <v>7</v>
@@ -2175,13 +2154,13 @@
         <v>19</v>
       </c>
       <c r="AS1" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AT1" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AU1" s="16" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AV1" s="16" t="s">
         <v>54</v>
@@ -2217,58 +2196,58 @@
         <v>53</v>
       </c>
       <c r="BG1" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="BH1" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="BI1" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="BJ1" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="BK1" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="BL1" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="BM1" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="BH1" s="13" t="s">
+      <c r="BN1" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="BO1" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="BP1" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="BQ1" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="BR1" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="BS1" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="BI1" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="BJ1" s="13" t="s">
+      <c r="BT1" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="BK1" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="BL1" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="BM1" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="BN1" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="BO1" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="BP1" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="BQ1" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="BR1" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="BS1" s="13" t="s">
+      <c r="BU1" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="BT1" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="BU1" s="13" t="s">
-        <v>217</v>
-      </c>
       <c r="BV1" s="13" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="BW1" s="13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="BX1" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="BY1" s="13" t="s">
         <v>68</v>
@@ -2286,181 +2265,181 @@
         <v>72</v>
       </c>
       <c r="CD1" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="CE1" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="CF1" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="CG1" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="CE1" s="13" t="s">
+      <c r="CH1" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="CI1" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="CJ1" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="CK1" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="CL1" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="CM1" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="CF1" s="13" t="s">
+      <c r="CN1" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="CG1" s="13" t="s">
+      <c r="CO1" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="CP1" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="CQ1" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="CR1" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="CS1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="CT1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="CU1" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="CV1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="CW1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="CX1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="CY1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="CZ1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="DA1" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="CH1" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="CI1" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="CJ1" s="13" t="s">
+      <c r="DB1" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="DC1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="DD1" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="DE1" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="DF1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="DG1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="DH1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="DI1" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="DJ1" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="CK1" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="CL1" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="CM1" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="CN1" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="CO1" s="13" t="s">
+      <c r="DK1" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="DL1" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="CP1" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="CQ1" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="CR1" s="13" t="s">
+      <c r="DM1" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="CS1" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="CT1" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="CU1" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="CV1" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="CW1" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="CX1" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="CY1" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="CZ1" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="DA1" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="DB1" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="DC1" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="DD1" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="DE1" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="DF1" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="DG1" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="DH1" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="DI1" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="DJ1" s="13" t="s">
+      <c r="DN1" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="DO1" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="DP1" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="DQ1" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="DR1" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="DS1" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="DT1" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="DK1" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="DL1" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="DM1" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="DN1" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="DO1" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="DP1" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="DQ1" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="DR1" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="DS1" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="DT1" s="17" t="s">
+      <c r="DU1" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="DV1" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="DW1" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="DU1" s="17" t="s">
+      <c r="DX1" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="DV1" s="17" t="s">
+      <c r="DY1" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="DW1" s="17" t="s">
+      <c r="DZ1" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="DX1" s="17" t="s">
+      <c r="EA1" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="DY1" s="17" t="s">
+      <c r="EB1" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="DZ1" s="17" t="s">
+      <c r="EC1" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="EA1" s="17" t="s">
+      <c r="ED1" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="EE1" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="EB1" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="EC1" s="17" t="s">
+      <c r="EF1" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="ED1" s="17" t="s">
+      <c r="EG1" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="EH1" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="EE1" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="EF1" s="17" t="s">
+      <c r="EI1" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="EG1" s="17" t="s">
+      <c r="EJ1" s="17" t="s">
         <v>264</v>
-      </c>
-      <c r="EH1" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="EI1" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="EJ1" s="17" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:140" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -2468,13 +2447,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>0</v>
@@ -2489,7 +2468,7 @@
         <v>21</v>
       </c>
       <c r="R2" s="22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="S2" s="21" t="s">
         <v>20</v>
@@ -2507,13 +2486,13 @@
         <v>22</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AA2" s="21" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AB2" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AC2" s="21" t="s">
         <v>23</v>
@@ -2522,10 +2501,10 @@
         <v>28907</v>
       </c>
       <c r="AE2" s="18" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="AF2" s="18" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="AG2" s="21">
         <v>3015774089</v>
@@ -2564,13 +2543,13 @@
         <v>40</v>
       </c>
       <c r="AS2" s="21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AT2" s="21" t="s">
         <v>0</v>
       </c>
       <c r="AU2" s="21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="AV2" s="21" t="s">
         <v>37</v>
@@ -2624,10 +2603,10 @@
         <v>66</v>
       </c>
       <c r="BQ2" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="BR2" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="BS2" s="21" t="s">
         <v>67</v>
@@ -2639,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="BY2" s="21" t="s">
-        <v>76</v>
+        <v>432</v>
       </c>
       <c r="BZ2" s="21" t="s">
         <v>75</v>
@@ -2663,10 +2642,10 @@
         <v>0</v>
       </c>
       <c r="CG2" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CH2" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="CI2" s="21">
         <v>1997</v>
@@ -2675,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="CL2" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="CM2" s="21" t="s">
         <v>0</v>
@@ -2684,55 +2663,55 @@
         <v>0</v>
       </c>
       <c r="CO2" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="CQ2" s="21">
         <v>101</v>
       </c>
       <c r="CR2" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="CS2" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="CT2" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CU2" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CV2" s="21">
         <v>1985</v>
       </c>
       <c r="CX2" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="CY2" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="CY2" s="21" t="s">
-        <v>90</v>
-      </c>
       <c r="CZ2" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="DA2" s="21" t="s">
         <v>0</v>
       </c>
       <c r="DB2" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="DC2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="DD2" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="DD2" s="21" t="s">
+      <c r="DE2" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="DE2" s="21" t="s">
-        <v>114</v>
-      </c>
       <c r="DF2" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DG2" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DH2" s="21">
         <v>3028976789</v>
@@ -2741,31 +2720,31 @@
         <v>0</v>
       </c>
       <c r="DJ2" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK2" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL2" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM2" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL2" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM2" s="21" t="s">
+      <c r="DN2" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO2" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN2" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO2" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP2" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ2" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR2" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS2" s="21" t="s">
         <v>0</v>
@@ -2804,7 +2783,7 @@
         <v>0</v>
       </c>
       <c r="EE2" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF2" s="21" t="s">
         <v>0</v>
@@ -2827,16 +2806,16 @@
         <v>38</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="D3" s="21" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O3" s="21">
         <v>1920</v>
@@ -2848,28 +2827,28 @@
         <v>23</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="S3" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="X3" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y3" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE3" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="AF3" s="18" t="s">
         <v>145</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="X3" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="Y3" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="AE3" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="AF3" s="18" t="s">
-        <v>146</v>
       </c>
       <c r="AG3" s="21">
         <v>3015774089</v>
@@ -2884,7 +2863,7 @@
         <v>3014524258</v>
       </c>
       <c r="AK3" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AL3" s="21" t="s">
         <v>25</v>
@@ -2908,32 +2887,32 @@
         <v>40</v>
       </c>
       <c r="AS3" s="21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AT3" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BH3" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="BI3" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="BK3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL3" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="BI3" s="22" t="s">
-        <v>303</v>
-      </c>
-      <c r="BK3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL3" s="21" t="s">
+      <c r="BP3" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="BP3" s="21" t="s">
+      <c r="BS3" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="BS3" s="21" t="s">
-        <v>153</v>
-      </c>
       <c r="BT3" s="21" t="s">
         <v>0</v>
       </c>
@@ -2941,121 +2920,121 @@
         <v>0</v>
       </c>
       <c r="BY3" s="21" t="s">
-        <v>154</v>
+        <v>432</v>
       </c>
       <c r="BZ3" s="21" t="s">
         <v>75</v>
       </c>
       <c r="CA3" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="CB3" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CC3" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="CD3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CE3" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="CF3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CG3" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="CJ3" s="21">
         <v>100</v>
       </c>
       <c r="CK3" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CL3" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="CM3" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CN3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CO3" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="CP3" s="22" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="CR3" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="CS3" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="CT3" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="CW3" s="21">
         <v>102</v>
       </c>
       <c r="CX3" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="CY3" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="CZ3" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="CY3" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="CZ3" s="21" t="s">
-        <v>158</v>
-      </c>
       <c r="DA3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="DB3" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="DD3" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="DF3" s="21" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="DG3" s="21" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="DH3" s="21">
         <v>3028976789</v>
       </c>
       <c r="DI3" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DJ3" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK3" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL3" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM3" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL3" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM3" s="21" t="s">
+      <c r="DN3" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO3" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN3" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO3" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP3" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ3" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR3" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS3" s="21" t="s">
         <v>0</v>
@@ -3094,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="EE3" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF3" s="21" t="s">
         <v>0</v>
@@ -3117,16 +3096,16 @@
         <v>38</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O4" s="21">
         <v>1910</v>
@@ -3138,28 +3117,28 @@
         <v>21</v>
       </c>
       <c r="R4" s="22" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="S4" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T4" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="V4" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="V4" s="21" t="s">
-        <v>170</v>
-      </c>
       <c r="X4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Y4" s="21" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="AE4" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AF4" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AG4" s="21">
         <v>3015774089</v>
@@ -3174,7 +3153,7 @@
         <v>3015567865</v>
       </c>
       <c r="AK4" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL4" s="21" t="s">
         <v>27</v>
@@ -3183,25 +3162,25 @@
         <v>27</v>
       </c>
       <c r="AT4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BH4" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BK4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BL4" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="BP4" s="21" t="s">
         <v>66</v>
       </c>
       <c r="BS4" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="BT4" s="21" t="s">
         <v>0</v>
@@ -3210,82 +3189,82 @@
         <v>0</v>
       </c>
       <c r="BY4" s="21" t="s">
-        <v>175</v>
+        <v>432</v>
       </c>
       <c r="BZ4" s="21" t="s">
         <v>75</v>
       </c>
       <c r="CA4" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CB4" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CC4" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CD4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CE4" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="CF4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CG4" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="CK4" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="CL4" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CN4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CO4" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CR4" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="CS4" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="CT4" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="CX4" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="CF4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CG4" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="CK4" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="CL4" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="CM4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CN4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CO4" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="CR4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="CS4" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="CT4" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="CX4" s="21" t="s">
-        <v>177</v>
-      </c>
       <c r="CY4" s="21" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="CZ4" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="DA4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DB4" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="DC4" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="DD4" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="DA4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DB4" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="DC4" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="DD4" s="23" t="s">
-        <v>181</v>
-      </c>
       <c r="DF4" s="21" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="DG4" s="21" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="DH4" s="21">
         <v>3028976789</v>
@@ -3294,85 +3273,85 @@
         <v>0</v>
       </c>
       <c r="DJ4" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK4" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL4" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM4" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL4" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM4" s="21" t="s">
+      <c r="DN4" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO4" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN4" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO4" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP4" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ4" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR4" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DT4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DU4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DV4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DW4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DX4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DY4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DZ4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EA4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EB4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EC4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="ED4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EE4" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EG4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EH4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EI4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EJ4" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:140" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3380,16 +3359,16 @@
         <v>38</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O5" s="21">
         <v>1925</v>
@@ -3401,34 +3380,34 @@
         <v>21</v>
       </c>
       <c r="R5" s="22" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="S5" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="T5" s="21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="U5" s="21" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="V5" s="21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="W5" s="21" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="X5" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Y5" s="21" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AE5" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AF5" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AG5" s="21">
         <v>3015774089</v>
@@ -3443,19 +3422,19 @@
         <v>3015567865</v>
       </c>
       <c r="AK5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AT5" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BH5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BK5" s="21" t="s">
         <v>0</v>
@@ -3464,7 +3443,7 @@
         <v>31</v>
       </c>
       <c r="BM5" s="21" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="BP5" s="21" t="s">
         <v>66</v>
@@ -3479,85 +3458,85 @@
         <v>0</v>
       </c>
       <c r="BY5" s="21" t="s">
-        <v>364</v>
+        <v>432</v>
       </c>
       <c r="BZ5" s="21" t="s">
         <v>75</v>
       </c>
       <c r="CA5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CB5" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CC5" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="CD5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE5" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="CF5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CG5" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="CK5" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="CL5" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM5" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="CN5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="CO5" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="CD5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CE5" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="CF5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CG5" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="CK5" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="CL5" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="CM5" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="CN5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="CO5" s="21" t="s">
-        <v>150</v>
-      </c>
       <c r="CP5" s="22" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="CR5" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="CS5" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="CT5" s="21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="CX5" s="21" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="CY5" s="21" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="CZ5" s="21" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="DA5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="DB5" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="DD5" s="21" t="s">
         <v>37</v>
       </c>
       <c r="DE5" s="21" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="DF5" s="21" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="DG5" s="21" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="DH5" s="21">
         <v>3028976789</v>
@@ -3566,85 +3545,85 @@
         <v>0</v>
       </c>
       <c r="DJ5" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK5" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL5" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM5" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL5" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM5" s="21" t="s">
+      <c r="DN5" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO5" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN5" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO5" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP5" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ5" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR5" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DT5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DU5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DV5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DW5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DX5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DY5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DZ5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EA5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EB5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EC5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="ED5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EE5" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EG5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EH5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EI5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EJ5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:140" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3652,16 +3631,16 @@
         <v>38</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O6" s="21">
         <v>1950</v>
@@ -3673,28 +3652,28 @@
         <v>26</v>
       </c>
       <c r="R6" s="22" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="S6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="V6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="X6" s="21" t="s">
         <v>0</v>
       </c>
       <c r="Y6" s="21" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="AE6" s="18" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AF6" s="21" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AG6" s="21">
         <v>3015774089</v>
@@ -3709,144 +3688,147 @@
         <v>3015774089</v>
       </c>
       <c r="AK6" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AL6" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AT6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BG6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BI6" s="24"/>
       <c r="BK6" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BL6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BP6" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BS6" s="21" t="s">
         <v>67</v>
       </c>
       <c r="BT6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
+      </c>
+      <c r="BY6" s="21" t="s">
+        <v>432</v>
       </c>
       <c r="CF6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CP6" s="24"/>
       <c r="DA6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DB6" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="DC6" s="21" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="DD6" s="21" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="DE6" s="21" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="DF6" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DG6" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DH6" s="21">
         <v>3028976789</v>
       </c>
       <c r="DI6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DJ6" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK6" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL6" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM6" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL6" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM6" s="21" t="s">
+      <c r="DN6" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO6" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN6" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO6" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP6" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ6" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR6" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DT6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DU6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DV6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DW6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DX6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DY6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DZ6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EA6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EB6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EC6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="ED6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EE6" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EG6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EH6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EI6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EJ6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:140" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -3854,16 +3836,16 @@
         <v>38</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O7" s="21">
         <v>1940</v>
@@ -3875,28 +3857,28 @@
         <v>11</v>
       </c>
       <c r="R7" s="22" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="S7" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="T7" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="V7" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="X7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Y7" s="21" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AE7" s="18" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="AF7" s="18" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="AG7" s="21">
         <v>3015774089</v>
@@ -3911,16 +3893,16 @@
         <v>3014524258</v>
       </c>
       <c r="AK7" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AL7" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AT7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BI7" s="24"/>
       <c r="BK7" s="21" t="s">
@@ -3930,10 +3912,10 @@
         <v>31</v>
       </c>
       <c r="BM7" s="21" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="BN7" s="21" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="BO7" s="21" t="s">
         <v>0</v>
@@ -3948,68 +3930,71 @@
         <v>0</v>
       </c>
       <c r="BU7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BV7" s="21" t="s">
-        <v>373</v>
+        <v>369</v>
+      </c>
+      <c r="BY7" s="21" t="s">
+        <v>432</v>
       </c>
       <c r="CD7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CF7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CP7" s="24"/>
       <c r="DA7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DB7" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="DC7" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="DD7" s="21" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="DF7" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DG7" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DH7" s="21">
         <v>3028976789</v>
       </c>
       <c r="DI7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DJ7" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK7" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL7" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM7" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL7" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM7" s="21" t="s">
+      <c r="DN7" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO7" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN7" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO7" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP7" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ7" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR7" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS7" s="21" t="s">
         <v>0</v>
@@ -4048,7 +4033,7 @@
         <v>0</v>
       </c>
       <c r="EE7" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF7" s="21" t="s">
         <v>0</v>
@@ -4071,16 +4056,16 @@
         <v>38</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O8" s="21">
         <v>1930</v>
@@ -4092,31 +4077,31 @@
         <v>30</v>
       </c>
       <c r="R8" s="22" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="S8" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T8" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="V8" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="X8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Y8" s="21" t="s">
         <v>22</v>
       </c>
       <c r="Z8" s="21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AA8" s="21" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AB8" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AC8" s="21" t="s">
         <v>23</v>
@@ -4125,10 +4110,10 @@
         <v>28907</v>
       </c>
       <c r="AE8" s="18" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AF8" s="18" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AG8" s="21">
         <v>3015774089</v>
@@ -4143,78 +4128,81 @@
         <v>3015567865</v>
       </c>
       <c r="AK8" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL8" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AT8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BJ8" s="24"/>
       <c r="BK8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BT8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="BY8" s="21" t="s">
+        <v>432</v>
       </c>
       <c r="CF8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CP8" s="24"/>
       <c r="DA8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DB8" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="DD8" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DE8" s="21" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="DF8" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DG8" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DH8" s="21">
         <v>3028976789</v>
       </c>
       <c r="DI8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DJ8" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK8" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL8" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM8" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL8" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM8" s="21" t="s">
+      <c r="DN8" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO8" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN8" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO8" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP8" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ8" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR8" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS8" s="21" t="s">
         <v>0</v>
@@ -4253,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="EE8" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF8" s="21" t="s">
         <v>0</v>
@@ -4276,13 +4264,13 @@
         <v>38</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="N9" s="21" t="s">
         <v>0</v>
@@ -4297,28 +4285,28 @@
         <v>29</v>
       </c>
       <c r="R9" s="22" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="T9" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="V9" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="V9" s="21" t="s">
-        <v>170</v>
-      </c>
       <c r="X9" s="21" t="s">
         <v>0</v>
       </c>
       <c r="Y9" s="21" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="AE9" s="18" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="AF9" s="18" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="AG9" s="21">
         <v>3015774089</v>
@@ -4333,16 +4321,16 @@
         <v>3015567865</v>
       </c>
       <c r="AK9" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL9" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AT9" s="21" t="s">
         <v>0</v>
       </c>
       <c r="AU9" s="21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="AV9" s="21" t="s">
         <v>37</v>
@@ -4387,7 +4375,7 @@
         <v>119</v>
       </c>
       <c r="BK9" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BT9" s="21" t="s">
         <v>0</v>
@@ -4396,65 +4384,65 @@
         <v>0</v>
       </c>
       <c r="BY9" s="21" t="s">
-        <v>388</v>
+        <v>432</v>
       </c>
       <c r="BZ9" s="21" t="s">
         <v>75</v>
       </c>
       <c r="CA9" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CB9" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CC9" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CD9" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CF9" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CG9" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="CJ9" s="21">
         <v>102</v>
       </c>
       <c r="CK9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CL9" s="21" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="CM9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CN9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CP9" s="24"/>
       <c r="CR9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DA9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DB9" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="DC9" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="DD9" s="23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="DF9" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DG9" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DH9" s="21">
         <v>3028976789</v>
@@ -4463,111 +4451,111 @@
         <v>0</v>
       </c>
       <c r="DJ9" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK9" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL9" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM9" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL9" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM9" s="21" t="s">
+      <c r="DN9" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO9" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN9" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO9" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP9" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ9" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR9" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DT9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DU9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DV9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DW9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DX9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DY9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DZ9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EA9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EB9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EC9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="ED9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EE9" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EG9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EH9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EI9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EJ9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:140" s="21" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>0</v>
@@ -4585,7 +4573,7 @@
         <v>27</v>
       </c>
       <c r="R10" s="22" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="S10" s="21" t="s">
         <v>20</v>
@@ -4598,13 +4586,13 @@
         <v>22</v>
       </c>
       <c r="Z10" s="21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AA10" s="21" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AB10" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AC10" s="21" t="s">
         <v>23</v>
@@ -4613,10 +4601,10 @@
         <v>28907</v>
       </c>
       <c r="AE10" s="19" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AF10" s="18" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AG10" s="21">
         <v>3015774089</v>
@@ -4655,13 +4643,13 @@
         <v>40</v>
       </c>
       <c r="AS10" s="21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AT10" s="21" t="s">
         <v>0</v>
       </c>
       <c r="AU10" s="21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="AV10" s="21" t="s">
         <v>37</v>
@@ -4700,25 +4688,25 @@
         <v>0</v>
       </c>
       <c r="BH10" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BI10" s="22" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="BK10" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BL10" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="BP10" s="21" t="s">
         <v>66</v>
       </c>
       <c r="BQ10" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="BR10" s="23" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="BS10" s="21" t="s">
         <v>67</v>
@@ -4730,16 +4718,16 @@
         <v>0</v>
       </c>
       <c r="BY10" s="21" t="s">
-        <v>376</v>
+        <v>432</v>
       </c>
       <c r="BZ10" s="21" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="CA10" s="21" t="s">
         <v>73</v>
       </c>
       <c r="CB10" s="21" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="CC10" s="21" t="s">
         <v>73</v>
@@ -4754,10 +4742,10 @@
         <v>0</v>
       </c>
       <c r="CG10" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CH10" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="CI10" s="21">
         <v>1997</v>
@@ -4766,7 +4754,7 @@
         <v>0</v>
       </c>
       <c r="CL10" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="CM10" s="21" t="s">
         <v>0</v>
@@ -4775,55 +4763,55 @@
         <v>0</v>
       </c>
       <c r="CO10" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="CQ10" s="21">
         <v>103</v>
       </c>
       <c r="CR10" s="21" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="CS10" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="CT10" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CU10" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="CV10" s="21">
         <v>1985</v>
       </c>
       <c r="CX10" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="CY10" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="CY10" s="21" t="s">
-        <v>90</v>
-      </c>
       <c r="CZ10" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="DA10" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DB10" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="DC10" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="DD10" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="DD10" s="21" t="s">
+      <c r="DE10" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="DE10" s="21" t="s">
-        <v>114</v>
-      </c>
       <c r="DF10" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DG10" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DH10" s="21">
         <v>3028976789</v>
@@ -4832,31 +4820,31 @@
         <v>0</v>
       </c>
       <c r="DJ10" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK10" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL10" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM10" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL10" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM10" s="21" t="s">
+      <c r="DN10" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO10" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN10" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO10" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP10" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ10" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR10" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS10" s="21" t="s">
         <v>0</v>
@@ -4895,7 +4883,7 @@
         <v>0</v>
       </c>
       <c r="EE10" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF10" s="21" t="s">
         <v>0</v>
@@ -4915,37 +4903,37 @@
     </row>
     <row r="11" spans="1:140" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>48</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O11" s="21">
         <v>1935</v>
@@ -4957,22 +4945,22 @@
         <v>21</v>
       </c>
       <c r="R11" s="22" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="S11" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="X11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Y11" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AE11" s="18" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AF11" s="19" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AG11" s="21">
         <v>3015774089</v>
@@ -4987,33 +4975,33 @@
         <v>3014524258</v>
       </c>
       <c r="AK11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AT11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BG11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BH11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BI11" s="24"/>
       <c r="BK11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BL11" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP11" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="BP11" s="21" t="s">
+      <c r="BS11" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="BS11" s="21" t="s">
-        <v>153</v>
-      </c>
       <c r="BT11" s="21" t="s">
         <v>0</v>
       </c>
@@ -5021,83 +5009,83 @@
         <v>0</v>
       </c>
       <c r="BY11" s="21" t="s">
-        <v>394</v>
+        <v>432</v>
       </c>
       <c r="BZ11" s="21" t="s">
         <v>75</v>
       </c>
       <c r="CA11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CB11" s="21" t="s">
         <v>74</v>
       </c>
       <c r="CC11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CD11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CE11" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="CF11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CG11" s="21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="CK11" s="21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="CL11" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="CM11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CN11" s="21" t="s">
         <v>0</v>
       </c>
       <c r="CO11" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="CP11" s="24"/>
       <c r="CR11" s="21" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="CS11" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="CT11" s="21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="CX11" s="21" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="CY11" s="21" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="CZ11" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="DA11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="DB11" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="DC11" s="21" t="s">
+        <v>385</v>
+      </c>
+      <c r="DD11" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="DA11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="DB11" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="DC11" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="DD11" s="21" t="s">
-        <v>181</v>
-      </c>
       <c r="DF11" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DG11" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DH11" s="21">
         <v>3028976789</v>
@@ -5106,117 +5094,117 @@
         <v>0</v>
       </c>
       <c r="DJ11" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK11" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL11" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM11" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL11" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM11" s="21" t="s">
+      <c r="DN11" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO11" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN11" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO11" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP11" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ11" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR11" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DT11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DU11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DV11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DW11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DX11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DY11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DZ11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EA11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EB11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EC11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="ED11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EE11" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EG11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EH11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EI11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EJ11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:140" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="M12" s="21" t="s">
         <v>0</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O12" s="21">
         <v>1930</v>
@@ -5228,22 +5216,22 @@
         <v>30</v>
       </c>
       <c r="R12" s="22" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="S12" s="21" t="s">
         <v>20</v>
       </c>
       <c r="X12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Y12" s="21" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="AE12" s="19" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="AF12" s="19" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="AG12" s="21">
         <v>3015774089</v>
@@ -5258,44 +5246,47 @@
         <v>3014524258</v>
       </c>
       <c r="AK12" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AL12" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AT12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BK12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BT12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="BY12" s="21" t="s">
+        <v>432</v>
       </c>
       <c r="CF12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="CP12" s="24"/>
       <c r="DA12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DB12" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="DC12" s="21" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="DD12" s="21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="DF12" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="DG12" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="DH12" s="21">
         <v>3028976789</v>
@@ -5304,117 +5295,117 @@
         <v>0</v>
       </c>
       <c r="DJ12" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK12" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL12" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM12" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL12" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM12" s="21" t="s">
+      <c r="DN12" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO12" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN12" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO12" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP12" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ12" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR12" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DT12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DU12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DV12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DW12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DX12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DY12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="DZ12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EA12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EB12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EC12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="ED12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EE12" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EG12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EH12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EI12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="EJ12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:140" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O13" s="21">
         <v>1940</v>
@@ -5426,22 +5417,22 @@
         <v>21</v>
       </c>
       <c r="R13" s="22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="S13" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="X13" s="21" t="s">
         <v>0</v>
       </c>
       <c r="Y13" s="21" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="AE13" s="19" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="AF13" s="19" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="AG13" s="21">
         <v>3015774089</v>
@@ -5456,28 +5447,28 @@
         <v>3014524258</v>
       </c>
       <c r="AK13" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AL13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AT13" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BG13" s="21" t="s">
         <v>0</v>
       </c>
       <c r="BH13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BY13" s="21" t="s">
-        <v>393</v>
+        <v>432</v>
       </c>
       <c r="BZ13" s="21" t="s">
         <v>75</v>
       </c>
       <c r="CA13" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="CB13" s="21" t="s">
         <v>74</v>
@@ -5492,129 +5483,129 @@
         <v>67</v>
       </c>
       <c r="DJ13" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="DK13" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL13" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM13" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="DL13" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM13" s="21" t="s">
+      <c r="DN13" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DO13" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="DN13" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="DO13" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="DP13" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DQ13" s="21" t="s">
         <v>48</v>
       </c>
       <c r="DR13" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="DS13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DT13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DU13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DV13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DW13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DX13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DY13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DZ13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EA13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EB13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EC13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="ED13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EE13" s="27" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="EF13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EG13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EH13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EI13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="EJ13" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:140" s="21" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="25" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="AE14" s="19" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="AF14" s="19" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:140" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K15" s="21" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="AE15" s="19" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="AF15" s="19" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16" spans="1:140" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K16" s="21" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="AE16" s="19" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="AF16" s="19" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="11:32" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="K17" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE17" s="19" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="AF17" s="19" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" spans="11:32" s="21" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -5677,34 +5668,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>285</v>
-      </c>
       <c r="H1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>128</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5712,7 +5703,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>60</v>
@@ -5741,10 +5732,10 @@
         <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>62</v>
@@ -5765,7 +5756,7 @@
         <v>1991</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5773,19 +5764,19 @@
         <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="4">
         <v>3013454562</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
@@ -5797,7 +5788,7 @@
         <v>1992</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5805,19 +5796,19 @@
         <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E5" s="4">
         <v>3013454562</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
@@ -5829,7 +5820,7 @@
         <v>1993</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5837,19 +5828,19 @@
         <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E6" s="4">
         <v>3013454562</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
@@ -5861,7 +5852,7 @@
         <v>1994</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -5869,19 +5860,19 @@
         <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E7" s="4">
         <v>3013454562</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
@@ -5893,12 +5884,12 @@
         <v>1995</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I12" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -5928,51 +5919,51 @@
   <sheetData>
     <row r="1" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" s="2">
         <v>1965</v>
@@ -5982,27 +5973,27 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -6010,59 +6001,59 @@
         <v>90</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -6073,30 +6064,30 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>339</v>
-      </c>
       <c r="C6" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="20">
         <v>1965</v>
@@ -6106,27 +6097,27 @@
         <v>0</v>
       </c>
       <c r="H6" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="K6" s="20" t="s">
         <v>343</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>344</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>340</v>
-      </c>
       <c r="C7" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -6134,59 +6125,59 @@
         <v>90</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H7" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="K7" s="20" t="s">
         <v>347</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>348</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>349</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H8" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="K8" s="20" t="s">
         <v>351</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>352</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>353</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
@@ -6197,16 +6188,16 @@
         <v>0</v>
       </c>
       <c r="H9" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>353</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="K9" s="20" t="s">
         <v>355</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>356</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>357</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>